<commit_message>
Pulizia repository + aggiunta file supporto mercato
- Spostati file MD in MD_SVILUPPO/ per migliore organizzazione
- Aggiunti file Excel mercato in Mercato/
- Aggiunti asset documento BP in assets/
- Aggiornati package.json e layout
- Aggiunti componenti utility (DatabaseSyncIndicator, MercatoDataLoader, etc)
- Aggiunti types TypeScript per ecografi e mercato
- File temporanei Excel rimossi
- Struttura repository ora pulita e organizzata
</commit_message>
<xml_diff>
--- a/assets/Eco_ITA_MASTER.xlsx
+++ b/assets/Eco_ITA_MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dracs/Documents/START_UP/DOC PROGETTI/DOC_ECO 3d Multisonda/__BP 2025/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EC01409-C863-C642-89A8-735BC2409E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6BB232-5469-BD40-AC98-A7FAE054BC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29820" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ECO_Riepilogo" sheetId="2" r:id="rId1"/>
@@ -724,7 +724,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="196">
   <si>
     <t>PRIORITÀ U</t>
   </si>
@@ -1253,6 +1253,114 @@
   <si>
     <t>Stima annua SSN</t>
   </si>
+  <si>
+    <t>Mercato di riferimento</t>
+  </si>
+  <si>
+    <t>Volume esami (x Italia)</t>
+  </si>
+  <si>
+    <t>Valore economico (x Italia)</t>
+  </si>
+  <si>
+    <t>Quota Italia (%)</t>
+  </si>
+  <si>
+    <r>
+      <t>USA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 🇺🇸</t>
+    </r>
+  </si>
+  <si>
+    <t>× 8 – 10</t>
+  </si>
+  <si>
+    <t>× 6 – 8</t>
+  </si>
+  <si>
+    <t>~10–12 %</t>
+  </si>
+  <si>
+    <r>
+      <t>Europa (UE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 🇪🇺</t>
+    </r>
+  </si>
+  <si>
+    <t>× 7 – 8</t>
+  </si>
+  <si>
+    <t>× 6 – 7</t>
+  </si>
+  <si>
+    <t>~12–15 %</t>
+  </si>
+  <si>
+    <r>
+      <t>Cina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 🇨🇳</t>
+    </r>
+  </si>
+  <si>
+    <t>× 10 – 12</t>
+  </si>
+  <si>
+    <t>× 9 – 11</t>
+  </si>
+  <si>
+    <t>~8–10 %</t>
+  </si>
+  <si>
+    <r>
+      <t>Globale</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 🌍</t>
+    </r>
+  </si>
+  <si>
+    <t>× 50 – 60</t>
+  </si>
+  <si>
+    <t>× 45 – 55</t>
+  </si>
+  <si>
+    <t>~1,5–2 %</t>
+  </si>
 </sst>
 </file>
 
@@ -1431,7 +1539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1476,6 +1584,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1845,11 +1954,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2854,14 +2963,14 @@
       </c>
       <c r="F54" s="9">
         <f>SUM(E54,G54)</f>
-        <v>1439429.8857142858</v>
+        <v>1367458.3914285717</v>
       </c>
       <c r="G54" s="9">
         <f>IFERROR((E54/100)*H54,"")</f>
-        <v>719714.94285714289</v>
+        <v>647743.44857142866</v>
       </c>
       <c r="H54" s="12">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -3065,13 +3174,83 @@
       </c>
       <c r="F69" s="10">
         <f>SUM(F6,F10,F14,F18,F22,F26,F30,F34,F38,F42,F46,F50,F54,F58,F62,)</f>
-        <v>15879246.483571425</v>
+        <v>15807274.989285711</v>
       </c>
       <c r="G69" s="10">
         <f>SUM(G6,G10,G14,G18,G22,G26,G30,G34,G38,G42,G46,G50,G54,G58,G62,)</f>
-        <v>5532987.1421428574</v>
+        <v>5461015.6478571435</v>
       </c>
       <c r="H69" s="12"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" t="s">
+        <v>182</v>
+      </c>
+      <c r="D73" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74" t="s">
+        <v>185</v>
+      </c>
+      <c r="C74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" t="s">
+        <v>189</v>
+      </c>
+      <c r="C75" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B76" t="s">
+        <v>193</v>
+      </c>
+      <c r="C76" t="s">
+        <v>194</v>
+      </c>
+      <c r="D76" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>